<commit_message>
resolviendo los errores enviados por mail
</commit_message>
<xml_diff>
--- a/data/output/Pedido_Semana_07_15022026_tierras_aridos.xlsx
+++ b/data/output/Pedido_Semana_07_15022026_tierras_aridos.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U57"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -705,7 +705,7 @@
         </is>
       </c>
       <c r="F3" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G3" s="4" t="n">
         <v>0</v>
@@ -720,7 +720,7 @@
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>AUMENTAR 30%</t>
         </is>
       </c>
       <c r="K3" s="3" t="n">
@@ -740,7 +740,7 @@
         <v>0</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R3" s="2" t="n">
         <v>0</v>
@@ -752,23 +752,23 @@
         <v>0</v>
       </c>
       <c r="U3" s="8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" hidden="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>3101010002</t>
+          <t>3201010001</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>COMPO SANA CONFORT</t>
+          <t>TURBA RUBIA</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">25L      </t>
+          <t xml:space="preserve">5L       </t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -782,13 +782,13 @@
         </is>
       </c>
       <c r="F4" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>12.65</v>
+        <v>6.62</v>
       </c>
       <c r="H4" s="4" t="n">
-        <v>5.06</v>
+        <v>2.65</v>
       </c>
       <c r="I4" s="5" t="inlineStr">
         <is>
@@ -797,28 +797,28 @@
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>AUMENTAR 30%</t>
         </is>
       </c>
       <c r="K4" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="6" t="n">
-        <v>63.25</v>
+        <v>6.62</v>
       </c>
       <c r="N4" s="4" t="n">
-        <v>37.95</v>
+        <v>3.97</v>
       </c>
       <c r="O4" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
+          <t xml:space="preserve">COMERCIAL QUIMICA MASSO S.A.                                                                                            </t>
         </is>
       </c>
       <c r="P4" s="3" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="3" t="n">
         <v>0</v>
@@ -827,10 +827,10 @@
         <v>0</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T4" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U4" s="8" t="n">
         <v>0</v>
@@ -849,7 +849,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">12L      </t>
+          <t xml:space="preserve">25L      </t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -863,35 +863,35 @@
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>8.050000000000001</v>
+        <v>12.65</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>3.22</v>
+        <v>5.06</v>
       </c>
       <c r="I5" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 15%</t>
         </is>
       </c>
       <c r="K5" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="6" t="n">
-        <v>24.15</v>
+        <v>63.25</v>
       </c>
       <c r="N5" s="4" t="n">
-        <v>14.49</v>
+        <v>37.95</v>
       </c>
       <c r="O5" s="7" t="inlineStr">
         <is>
@@ -899,19 +899,19 @@
         </is>
       </c>
       <c r="P5" s="3" t="n">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="Q5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R5" s="2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T5" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U5" s="8" t="n">
         <v>0</v>
@@ -920,17 +920,17 @@
     <row r="6" hidden="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>3101010003</t>
+          <t>3101010002</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>COMPO SANA UNIVERSAL</t>
+          <t>COMPO SANA CONFORT</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">80L      </t>
+          <t xml:space="preserve">12L      </t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -944,35 +944,35 @@
         </is>
       </c>
       <c r="F6" s="3" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>25.7</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="H6" s="4" t="n">
-        <v>10.28</v>
+        <v>3.22</v>
       </c>
       <c r="I6" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K6" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="6" t="n">
-        <v>179.9</v>
+        <v>24.15</v>
       </c>
       <c r="N6" s="4" t="n">
-        <v>107.94</v>
+        <v>14.49</v>
       </c>
       <c r="O6" s="7" t="inlineStr">
         <is>
@@ -980,16 +980,16 @@
         </is>
       </c>
       <c r="P6" s="3" t="n">
-        <v>37</v>
+        <v>137</v>
       </c>
       <c r="Q6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S6" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" s="3" t="n">
         <v>0</v>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">20L      </t>
+          <t xml:space="preserve">80L      </t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
@@ -1028,32 +1028,32 @@
         <v>6</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>9.800000000000001</v>
+        <v>25.7</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>3.92</v>
+        <v>10.28</v>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K7" s="3" t="n">
         <v>2</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>58.8</v>
+        <v>154.2</v>
       </c>
       <c r="N7" s="4" t="n">
-        <v>35.28</v>
+        <v>92.52</v>
       </c>
       <c r="O7" s="7" t="inlineStr">
         <is>
@@ -1061,13 +1061,13 @@
         </is>
       </c>
       <c r="P7" s="3" t="n">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="Q7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R7" s="2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S7" s="2" t="n">
         <v>0</v>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">40L      </t>
+          <t xml:space="preserve">20L      </t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -1106,35 +1106,35 @@
         </is>
       </c>
       <c r="F8" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>15.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>6.32</v>
+        <v>3.92</v>
       </c>
       <c r="I8" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K8" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>47.4</v>
+        <v>49</v>
       </c>
       <c r="N8" s="4" t="n">
-        <v>28.44</v>
+        <v>29.4</v>
       </c>
       <c r="O8" s="7" t="inlineStr">
         <is>
@@ -1142,16 +1142,16 @@
         </is>
       </c>
       <c r="P8" s="3" t="n">
-        <v>170</v>
+        <v>89</v>
       </c>
       <c r="Q8" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S8" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8" s="3" t="n">
         <v>0</v>
@@ -1163,22 +1163,22 @@
     <row r="9" hidden="1">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>3102010001</t>
+          <t>3101010003</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>COMPO BIO HUERTO CITRICOS 20L</t>
+          <t>COMPO SANA UNIVERSAL</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>         </t>
+          <t xml:space="preserve">40L      </t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>        </t>
+          <t xml:space="preserve">UNICO   </t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
@@ -1187,35 +1187,35 @@
         </is>
       </c>
       <c r="F9" s="3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>12.15</v>
+        <v>15.8</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>4.86</v>
+        <v>6.32</v>
       </c>
       <c r="I9" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K9" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M9" s="6" t="n">
-        <v>60.75</v>
+        <v>47.4</v>
       </c>
       <c r="N9" s="4" t="n">
-        <v>36.45</v>
+        <v>28.44</v>
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="P9" s="3" t="n">
-        <v>89</v>
+        <v>170</v>
       </c>
       <c r="Q9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R9" s="2" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="S9" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T9" s="3" t="n">
         <v>0</v>
@@ -1244,22 +1244,22 @@
     <row r="10" hidden="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>3102050001</t>
+          <t>3102010001</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>COMPO BIO HUERTO URBANO</t>
+          <t>COMPO BIO HUERTO CITRICOS 20L</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">50L      </t>
+          <t>         </t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">UNICO   </t>
+          <t>        </t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
@@ -1268,35 +1268,35 @@
         </is>
       </c>
       <c r="F10" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="I10" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 5%</t>
+        </is>
+      </c>
+      <c r="K10" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="4" t="n">
-        <v>23.03</v>
-      </c>
-      <c r="H10" s="4" t="n">
-        <v>9.210000000000001</v>
-      </c>
-      <c r="I10" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J10" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K10" s="3" t="n">
-        <v>1</v>
-      </c>
       <c r="L10" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M10" s="6" t="n">
-        <v>46.05</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="N10" s="4" t="n">
-        <v>27.63</v>
+        <v>43.74</v>
       </c>
       <c r="O10" s="7" t="inlineStr">
         <is>
@@ -1304,16 +1304,16 @@
         </is>
       </c>
       <c r="P10" s="3" t="n">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="Q10" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R10" s="2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="S10" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T10" s="3" t="n">
         <v>0</v>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">20L      </t>
+          <t xml:space="preserve">50L      </t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -1352,19 +1352,19 @@
         <v>2</v>
       </c>
       <c r="G11" s="4" t="n">
-        <v>11.2</v>
+        <v>23.03</v>
       </c>
       <c r="H11" s="4" t="n">
-        <v>4.48</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="I11" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K11" s="3" t="n">
@@ -1374,10 +1374,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="6" t="n">
-        <v>22.4</v>
+        <v>46.05</v>
       </c>
       <c r="N11" s="4" t="n">
-        <v>13.44</v>
+        <v>27.63</v>
       </c>
       <c r="O11" s="7" t="inlineStr">
         <is>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="P11" s="3" t="n">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="Q11" s="3" t="n">
         <v>0</v>
@@ -1394,10 +1394,10 @@
         <v>1</v>
       </c>
       <c r="S11" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T11" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" s="8" t="n">
         <v>0</v>
@@ -1406,22 +1406,22 @@
     <row r="12" hidden="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>3102060001</t>
+          <t>3102050001</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>COMPO SANA HORTENSIAS-AZALEAS 20L</t>
+          <t>COMPO BIO HUERTO URBANO</t>
         </is>
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>         </t>
+          <t xml:space="preserve">20L      </t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>        </t>
+          <t xml:space="preserve">UNICO   </t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
@@ -1430,52 +1430,52 @@
         </is>
       </c>
       <c r="F12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>4.48</v>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J12" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="N12" s="4" t="n">
+        <v>6.72</v>
+      </c>
+      <c r="O12" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
+        </is>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="Q12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" s="2" t="n">
         <v>2</v>
-      </c>
-      <c r="G12" s="4" t="n">
-        <v>10.1</v>
-      </c>
-      <c r="H12" s="4" t="n">
-        <v>4.04</v>
-      </c>
-      <c r="I12" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J12" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6" t="n">
-        <v>20.2</v>
-      </c>
-      <c r="N12" s="4" t="n">
-        <v>12.12</v>
-      </c>
-      <c r="O12" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
-        </is>
-      </c>
-      <c r="P12" s="3" t="n">
-        <v>95</v>
-      </c>
-      <c r="Q12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="S12" s="2" t="n">
-        <v>3</v>
       </c>
       <c r="T12" s="3" t="n">
         <v>1</v>
@@ -1487,12 +1487,12 @@
     <row r="13" hidden="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>3102100001</t>
+          <t>3102060001</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>COMPO SANA SEMILLEROS 20L</t>
+          <t>COMPO SANA HORTENSIAS-AZALEAS 20L</t>
         </is>
       </c>
       <c r="C13" s="2" t="inlineStr">
@@ -1511,69 +1511,69 @@
         </is>
       </c>
       <c r="F13" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G13" s="4" t="n">
-        <v>10.93</v>
+        <v>10.1</v>
       </c>
       <c r="H13" s="4" t="n">
-        <v>4.37</v>
+        <v>4.04</v>
       </c>
       <c r="I13" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J13" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="6" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="N13" s="4" t="n">
+        <v>12.12</v>
+      </c>
+      <c r="O13" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
+        </is>
+      </c>
+      <c r="P13" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2" t="n">
         <v>2</v>
-      </c>
-      <c r="L13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="6" t="n">
-        <v>65.55</v>
-      </c>
-      <c r="N13" s="4" t="n">
-        <v>39.33</v>
-      </c>
-      <c r="O13" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
-        </is>
-      </c>
-      <c r="P13" s="3" t="n">
-        <v>56</v>
-      </c>
-      <c r="Q13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" s="2" t="n">
-        <v>6</v>
       </c>
       <c r="S13" s="2" t="n">
         <v>3</v>
       </c>
       <c r="T13" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="8" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>3103010002</t>
+          <t>3102100001</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>COMPO SANA CACTUS 5L</t>
+          <t>COMPO SANA SEMILLEROS 20L</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
@@ -1592,236 +1592,236 @@
         </is>
       </c>
       <c r="F14" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>10.93</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <v>4.37</v>
+      </c>
+      <c r="I14" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J14" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6" t="n">
+        <v>54.62</v>
+      </c>
+      <c r="N14" s="4" t="n">
+        <v>32.77</v>
+      </c>
+      <c r="O14" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
+        </is>
+      </c>
+      <c r="P14" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="Q14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="S14" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="G14" s="4" t="n">
-        <v>5.55</v>
-      </c>
-      <c r="H14" s="4" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="I14" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J14" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K14" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" s="6" t="n">
-        <v>16.65</v>
-      </c>
-      <c r="N14" s="4" t="n">
-        <v>9.99</v>
-      </c>
-      <c r="O14" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
-        </is>
-      </c>
-      <c r="P14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="R14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" s="2" t="n">
-        <v>4</v>
-      </c>
       <c r="T14" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U14" s="8" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
+          <t>3103010002</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>COMPO SANA CACTUS 5L</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>         </t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>        </t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>tierras_aridos</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="4" t="n">
+        <v>5.55</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="I15" s="5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J15" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K15" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="6" t="n">
+        <v>16.65</v>
+      </c>
+      <c r="N15" s="4" t="n">
+        <v>9.99</v>
+      </c>
+      <c r="O15" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
+        </is>
+      </c>
+      <c r="P15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="T15" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="U15" s="8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
           <t>3103030001</t>
         </is>
       </c>
-      <c r="B15" s="2" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>COMPO SANA ORQUIDEAS 5L</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>         </t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="D16" s="2" t="inlineStr">
         <is>
           <t>        </t>
         </is>
       </c>
-      <c r="E15" s="2" t="inlineStr">
+      <c r="E16" s="2" t="inlineStr">
         <is>
           <t>tierras_aridos</t>
         </is>
       </c>
-      <c r="F15" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="4" t="n">
+      <c r="F16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="n">
         <v>5.7</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H16" s="4" t="n">
         <v>2.28</v>
       </c>
-      <c r="I15" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J15" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K15" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="6" t="n">
+      <c r="I16" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J16" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 15%</t>
+        </is>
+      </c>
+      <c r="K16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6" t="n">
         <v>5.7</v>
       </c>
-      <c r="N15" s="4" t="n">
+      <c r="N16" s="4" t="n">
         <v>3.42</v>
       </c>
-      <c r="O15" s="7" t="inlineStr">
+      <c r="O16" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
         </is>
       </c>
-      <c r="P15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="3" t="n">
+      <c r="P16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="R15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U15" s="8" t="n">
+      <c r="R16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" s="8" t="n">
         <v>2</v>
-      </c>
-    </row>
-    <row r="16" hidden="1">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>3103040001</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>COMPO SANA PLANTAS VERDES</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">10L      </t>
-        </is>
-      </c>
-      <c r="D16" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">UNICO   </t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="inlineStr">
-        <is>
-          <t>tierras_aridos</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="G16" s="4" t="n">
-        <v>6.2</v>
-      </c>
-      <c r="H16" s="4" t="n">
-        <v>2.48</v>
-      </c>
-      <c r="I16" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J16" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K16" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="L16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" s="6" t="n">
-        <v>24.8</v>
-      </c>
-      <c r="N16" s="4" t="n">
-        <v>14.88</v>
-      </c>
-      <c r="O16" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
-        </is>
-      </c>
-      <c r="P16" s="3" t="n">
-        <v>28</v>
-      </c>
-      <c r="Q16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="T16" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="U16" s="8" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="17" hidden="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>3203050002</t>
+          <t>3103040001</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>BIG BAG CANTO RODADO BLANCO 500KG</t>
+          <t>COMPO SANA PLANTAS VERDES</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">40I60    </t>
+          <t xml:space="preserve">10L      </t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
@@ -1835,55 +1835,55 @@
         </is>
       </c>
       <c r="F17" s="3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G17" s="4" t="n">
-        <v>162.67</v>
+        <v>6.2</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>65.06999999999999</v>
+        <v>2.48</v>
       </c>
       <c r="I17" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J17" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>AUMENTAR 19%</t>
         </is>
       </c>
       <c r="K17" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L17" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M17" s="6" t="n">
-        <v>162.67</v>
+        <v>31</v>
       </c>
       <c r="N17" s="4" t="n">
-        <v>97.59999999999999</v>
+        <v>18.6</v>
       </c>
       <c r="O17" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENVASADOS ARISAC SL                                                                                                     </t>
+          <t xml:space="preserve">COMPO IBERIA, S.L.                                                                                                      </t>
         </is>
       </c>
       <c r="P17" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="Q17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S17" s="2" t="n">
-        <v>0</v>
-      </c>
       <c r="T17" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U17" s="8" t="n">
         <v>0</v>
@@ -1892,22 +1892,22 @@
     <row r="18" hidden="1">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>3203050018</t>
+          <t>3203050002</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>ROCALLA NEGRA MUSGO X 1KG</t>
+          <t>BIG BAG CANTO RODADO BLANCO 500KG</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>         </t>
+          <t xml:space="preserve">40I60    </t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>        </t>
+          <t xml:space="preserve">UNICO   </t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
@@ -1916,35 +1916,35 @@
         </is>
       </c>
       <c r="F18" s="3" t="n">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="G18" s="4" t="n">
-        <v>0.55</v>
+        <v>162.67</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>0.22</v>
+        <v>65.06999999999999</v>
       </c>
       <c r="I18" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J18" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K18" s="3" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="L18" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M18" s="6" t="n">
-        <v>46.75</v>
+        <v>162.67</v>
       </c>
       <c r="N18" s="4" t="n">
-        <v>28.05</v>
+        <v>97.59999999999999</v>
       </c>
       <c r="O18" s="7" t="inlineStr">
         <is>
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="P18" s="3" t="n">
-        <v>857</v>
+        <v>2</v>
       </c>
       <c r="Q18" s="3" t="n">
         <v>0</v>
@@ -1973,22 +1973,22 @@
     <row r="19" hidden="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>3203050022</t>
+          <t>3203050018</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>SACO CANTO RODADO BLANCO 20KG</t>
+          <t>ROCALLA NEGRA MUSGO X 1KG</t>
         </is>
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">40I60    </t>
+          <t>         </t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">UNICO   </t>
+          <t>        </t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
@@ -1997,35 +1997,35 @@
         </is>
       </c>
       <c r="F19" s="3" t="n">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="G19" s="4" t="n">
-        <v>7.52</v>
+        <v>0.55</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>3.01</v>
+        <v>0.22</v>
       </c>
       <c r="I19" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J19" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K19" s="3" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="L19" s="3" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M19" s="6" t="n">
-        <v>75.25</v>
+        <v>42.9</v>
       </c>
       <c r="N19" s="4" t="n">
-        <v>45.15</v>
+        <v>25.74</v>
       </c>
       <c r="O19" s="7" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         </is>
       </c>
       <c r="P19" s="3" t="n">
-        <v>80</v>
+        <v>857</v>
       </c>
       <c r="Q19" s="3" t="n">
         <v>0</v>
@@ -2054,17 +2054,17 @@
     <row r="20" hidden="1">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>3203050025</t>
+          <t>3203050022</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>SACO GRAVA VOLCANICA MARRON 15KG</t>
+          <t>SACO CANTO RODADO BLANCO 20KG</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">5I10     </t>
+          <t xml:space="preserve">40I60    </t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
@@ -2078,35 +2078,35 @@
         </is>
       </c>
       <c r="F20" s="3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G20" s="4" t="n">
-        <v>4.68</v>
+        <v>7.52</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>1.87</v>
+        <v>3.01</v>
       </c>
       <c r="I20" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J20" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K20" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L20" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M20" s="6" t="n">
-        <v>18.7</v>
+        <v>67.72</v>
       </c>
       <c r="N20" s="4" t="n">
-        <v>11.22</v>
+        <v>40.63</v>
       </c>
       <c r="O20" s="7" t="inlineStr">
         <is>
@@ -2114,7 +2114,7 @@
         </is>
       </c>
       <c r="P20" s="3" t="n">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="Q20" s="3" t="n">
         <v>0</v>
@@ -2123,10 +2123,10 @@
         <v>0</v>
       </c>
       <c r="S20" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T20" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U20" s="8" t="n">
         <v>0</v>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">10I25    </t>
+          <t xml:space="preserve">5I10     </t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
@@ -2159,7 +2159,7 @@
         </is>
       </c>
       <c r="F21" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" s="4" t="n">
         <v>4.68</v>
@@ -2169,25 +2169,25 @@
       </c>
       <c r="I21" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J21" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K21" s="3" t="n">
         <v>1</v>
       </c>
       <c r="L21" s="3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M21" s="6" t="n">
-        <v>9.35</v>
+        <v>14.03</v>
       </c>
       <c r="N21" s="4" t="n">
-        <v>5.61</v>
+        <v>8.42</v>
       </c>
       <c r="O21" s="7" t="inlineStr">
         <is>
@@ -2195,7 +2195,7 @@
         </is>
       </c>
       <c r="P21" s="3" t="n">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="Q21" s="3" t="n">
         <v>0</v>
@@ -2204,10 +2204,10 @@
         <v>0</v>
       </c>
       <c r="S21" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T21" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U21" s="8" t="n">
         <v>0</v>
@@ -2216,17 +2216,17 @@
     <row r="22" hidden="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>3203050027</t>
+          <t>3203050025</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>SACO MARMOLINA BLANCA 20KG</t>
+          <t>SACO GRAVA VOLCANICA MARRON 15KG</t>
         </is>
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">9I12     </t>
+          <t xml:space="preserve">10I25    </t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
@@ -2243,19 +2243,19 @@
         <v>1</v>
       </c>
       <c r="G22" s="4" t="n">
-        <v>5.05</v>
+        <v>4.68</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>2.02</v>
+        <v>1.87</v>
       </c>
       <c r="I22" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J22" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K22" s="3" t="n">
@@ -2265,10 +2265,10 @@
         <v>0</v>
       </c>
       <c r="M22" s="6" t="n">
-        <v>5.05</v>
+        <v>4.68</v>
       </c>
       <c r="N22" s="4" t="n">
-        <v>3.03</v>
+        <v>2.81</v>
       </c>
       <c r="O22" s="7" t="inlineStr">
         <is>
@@ -2276,7 +2276,7 @@
         </is>
       </c>
       <c r="P22" s="3" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="Q22" s="3" t="n">
         <v>0</v>
@@ -2297,22 +2297,22 @@
     <row r="23" hidden="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>3203050019</t>
+          <t>3203050027</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>SACO ARENA RIO 15KG</t>
+          <t>SACO MARMOLINA BLANCA 20KG</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>         </t>
+          <t xml:space="preserve">9I12     </t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>        </t>
+          <t xml:space="preserve">UNICO   </t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">
@@ -2321,22 +2321,22 @@
         </is>
       </c>
       <c r="F23" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" s="4" t="n">
-        <v>0.98</v>
+        <v>5.05</v>
       </c>
       <c r="H23" s="4" t="n">
-        <v>0.39</v>
+        <v>2.02</v>
       </c>
       <c r="I23" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J23" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K23" s="3" t="n">
@@ -2346,24 +2346,24 @@
         <v>0</v>
       </c>
       <c r="M23" s="6" t="n">
-        <v>1.95</v>
+        <v>5.05</v>
       </c>
       <c r="N23" s="4" t="n">
-        <v>1.17</v>
+        <v>3.03</v>
       </c>
       <c r="O23" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">JOHNCLIMA GAS REGORMAS INTEGRALES S.L.                                                                                  </t>
+          <t xml:space="preserve">ENVASADOS ARISAC SL                                                                                                     </t>
         </is>
       </c>
       <c r="P23" s="3" t="n">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="Q23" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R23" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S23" s="2" t="n">
         <v>0</v>
@@ -2378,22 +2378,22 @@
     <row r="24" hidden="1">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>3101010006</t>
+          <t>3203050019</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>SUSTRATO PREMIUM</t>
+          <t>SACO ARENA RIO 15KG</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">25L      </t>
+          <t>         </t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">UNICO   </t>
+          <t>        </t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
@@ -2405,10 +2405,10 @@
         <v>1</v>
       </c>
       <c r="G24" s="4" t="n">
-        <v>11.23</v>
+        <v>0.98</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>4.49</v>
+        <v>0.39</v>
       </c>
       <c r="I24" s="5" t="inlineStr">
         <is>
@@ -2417,7 +2417,7 @@
       </c>
       <c r="J24" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 40%</t>
         </is>
       </c>
       <c r="K24" s="3" t="n">
@@ -2427,30 +2427,30 @@
         <v>0</v>
       </c>
       <c r="M24" s="6" t="n">
-        <v>11.23</v>
+        <v>0.98</v>
       </c>
       <c r="N24" s="4" t="n">
-        <v>6.74</v>
+        <v>0.59</v>
       </c>
       <c r="O24" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
+          <t xml:space="preserve">JOHNCLIMA GAS REGORMAS INTEGRALES S.L.                                                                                  </t>
         </is>
       </c>
       <c r="P24" s="3" t="n">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="Q24" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R24" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S24" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T24" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U24" s="8" t="n">
         <v>0</v>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">12L      </t>
+          <t xml:space="preserve">25L      </t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
@@ -2486,19 +2486,19 @@
         <v>1</v>
       </c>
       <c r="G25" s="4" t="n">
-        <v>6.7</v>
+        <v>11.23</v>
       </c>
       <c r="H25" s="4" t="n">
-        <v>2.68</v>
+        <v>4.49</v>
       </c>
       <c r="I25" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J25" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K25" s="3" t="n">
@@ -2508,10 +2508,10 @@
         <v>0</v>
       </c>
       <c r="M25" s="6" t="n">
-        <v>6.7</v>
+        <v>11.23</v>
       </c>
       <c r="N25" s="4" t="n">
-        <v>4.02</v>
+        <v>6.74</v>
       </c>
       <c r="O25" s="7" t="inlineStr">
         <is>
@@ -2519,19 +2519,19 @@
         </is>
       </c>
       <c r="P25" s="3" t="n">
-        <v>140</v>
+        <v>65</v>
       </c>
       <c r="Q25" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="S25" s="2" t="n">
-        <v>1</v>
-      </c>
       <c r="T25" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U25" s="8" t="n">
         <v>0</v>
@@ -2540,17 +2540,17 @@
     <row r="26" hidden="1">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>3101010007</t>
+          <t>3101010006</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>SUSTRATO UNIVERSAL BLUMENERDE</t>
+          <t>SUSTRATO PREMIUM</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">40L      </t>
+          <t xml:space="preserve">12L      </t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
@@ -2564,52 +2564,52 @@
         </is>
       </c>
       <c r="F26" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G26" s="4" t="n">
-        <v>7.92</v>
+        <v>6.7</v>
       </c>
       <c r="H26" s="4" t="n">
-        <v>3.17</v>
+        <v>2.68</v>
       </c>
       <c r="I26" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J26" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 9%</t>
         </is>
       </c>
       <c r="K26" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="6" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="N26" s="4" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="O26" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
+        </is>
+      </c>
+      <c r="P26" s="3" t="n">
+        <v>140</v>
+      </c>
+      <c r="Q26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L26" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" s="6" t="n">
-        <v>31.7</v>
-      </c>
-      <c r="N26" s="4" t="n">
-        <v>19.02</v>
-      </c>
-      <c r="O26" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
-        </is>
-      </c>
-      <c r="P26" s="3" t="n">
-        <v>189</v>
-      </c>
-      <c r="Q26" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" s="2" t="n">
-        <v>0</v>
-      </c>
       <c r="S26" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="3" t="n">
         <v>0</v>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">5L       </t>
+          <t xml:space="preserve">40L      </t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
@@ -2645,35 +2645,35 @@
         </is>
       </c>
       <c r="F27" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G27" s="4" t="n">
+        <v>7.92</v>
+      </c>
+      <c r="H27" s="4" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="I27" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J27" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K27" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G27" s="4" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="H27" s="4" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="I27" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J27" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K27" s="3" t="n">
-        <v>1</v>
-      </c>
       <c r="L27" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M27" s="6" t="n">
-        <v>2.75</v>
+        <v>31.7</v>
       </c>
       <c r="N27" s="4" t="n">
-        <v>1.65</v>
+        <v>19.02</v>
       </c>
       <c r="O27" s="7" t="inlineStr">
         <is>
@@ -2681,7 +2681,7 @@
         </is>
       </c>
       <c r="P27" s="3" t="n">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="Q27" s="3" t="n">
         <v>0</v>
@@ -2690,10 +2690,10 @@
         <v>0</v>
       </c>
       <c r="S27" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T27" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U27" s="8" t="n">
         <v>0</v>
@@ -2712,7 +2712,7 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">70L      </t>
+          <t xml:space="preserve">5L       </t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
@@ -2726,13 +2726,13 @@
         </is>
       </c>
       <c r="F28" s="3" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G28" s="4" t="n">
-        <v>0</v>
+        <v>1.38</v>
       </c>
       <c r="H28" s="4" t="n">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="I28" s="5" t="inlineStr">
         <is>
@@ -2741,40 +2741,40 @@
       </c>
       <c r="J28" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 40%</t>
         </is>
       </c>
       <c r="K28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="6" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="N28" s="4" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="O28" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
+        </is>
+      </c>
+      <c r="P28" s="3" t="n">
+        <v>164</v>
+      </c>
+      <c r="Q28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
-        </is>
-      </c>
-      <c r="P28" s="3" t="n">
-        <v>217</v>
-      </c>
-      <c r="Q28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="S28" s="2" t="n">
-        <v>1</v>
-      </c>
       <c r="T28" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U28" s="8" t="n">
         <v>0</v>
@@ -2783,149 +2783,149 @@
     <row r="29" hidden="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
+          <t>3101010007</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>SUSTRATO UNIVERSAL BLUMENERDE</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">70L      </t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UNICO   </t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>tierras_aridos</t>
+        </is>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J29" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K29" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
+        </is>
+      </c>
+      <c r="P29" s="3" t="n">
+        <v>217</v>
+      </c>
+      <c r="Q29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="S29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" hidden="1">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
           <t>3102070002</t>
         </is>
       </c>
-      <c r="B29" s="2" t="inlineStr">
+      <c r="B30" s="2" t="inlineStr">
         <is>
           <t>SUSTRATO CANABIUM  50L</t>
         </is>
       </c>
-      <c r="C29" s="2" t="inlineStr">
+      <c r="C30" s="2" t="inlineStr">
         <is>
           <t>         </t>
         </is>
       </c>
-      <c r="D29" s="2" t="inlineStr">
+      <c r="D30" s="2" t="inlineStr">
         <is>
           <t>        </t>
         </is>
       </c>
-      <c r="E29" s="2" t="inlineStr">
+      <c r="E30" s="2" t="inlineStr">
         <is>
           <t>tierras_aridos</t>
         </is>
       </c>
-      <c r="F29" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="4" t="n">
+      <c r="F30" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4" t="n">
         <v>12.52</v>
       </c>
-      <c r="H29" s="4" t="n">
+      <c r="H30" s="4" t="n">
         <v>5.01</v>
       </c>
-      <c r="I29" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J29" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K29" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" s="6" t="n">
+      <c r="I30" s="5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J30" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K30" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="6" t="n">
         <v>12.52</v>
       </c>
-      <c r="N29" s="4" t="n">
+      <c r="N30" s="4" t="n">
         <v>7.51</v>
       </c>
-      <c r="O29" s="7" t="inlineStr">
+      <c r="O30" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
         </is>
       </c>
-      <c r="P29" s="3" t="n">
+      <c r="P30" s="3" t="n">
         <v>108</v>
       </c>
-      <c r="Q29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U29" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>3103010003</t>
-        </is>
-      </c>
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>SUBSTRATO CACTUS 5L</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="inlineStr">
-        <is>
-          <t>         </t>
-        </is>
-      </c>
-      <c r="D30" s="2" t="inlineStr">
-        <is>
-          <t>        </t>
-        </is>
-      </c>
-      <c r="E30" s="2" t="inlineStr">
-        <is>
-          <t>tierras_aridos</t>
-        </is>
-      </c>
-      <c r="F30" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="4" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="H30" s="4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="I30" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J30" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K30" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L30" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" s="6" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="N30" s="4" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="O30" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
-        </is>
-      </c>
-      <c r="P30" s="3" t="n">
-        <v>2</v>
-      </c>
       <c r="Q30" s="3" t="n">
         <v>0</v>
       </c>
@@ -2933,24 +2933,24 @@
         <v>0</v>
       </c>
       <c r="S30" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T30" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U30" s="8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>3103030002</t>
+          <t>3103010003</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>SUBSTRATO ORQUIDEAS 5L</t>
+          <t>SUBSTRATO CACTUS 5L</t>
         </is>
       </c>
       <c r="C31" s="2" t="inlineStr">
@@ -2979,12 +2979,12 @@
       </c>
       <c r="I31" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="J31" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K31" s="3" t="n">
@@ -3005,346 +3005,346 @@
         </is>
       </c>
       <c r="P31" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="R31" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S31" s="2" t="n">
-        <v>1</v>
-      </c>
       <c r="T31" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U31" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>3103030002</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>SUBSTRATO ORQUIDEAS 5L</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>         </t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>        </t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>tierras_aridos</t>
+        </is>
+      </c>
+      <c r="F32" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="4" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="H32" s="4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I32" s="5" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="J32" s="2" t="inlineStr">
+        <is>
+          <t>AUMENTAR 30%</t>
+        </is>
+      </c>
+      <c r="K32" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="6" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="N32" s="4" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O32" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
+        </is>
+      </c>
+      <c r="P32" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="3" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" hidden="1">
-      <c r="A32" s="2" t="inlineStr">
+      <c r="R32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T32" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U32" s="8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" hidden="1">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>3103040002</t>
         </is>
       </c>
-      <c r="B32" s="2" t="inlineStr">
+      <c r="B33" s="2" t="inlineStr">
         <is>
           <t>SUBSTRATO PLANTAS VERDES 10L</t>
         </is>
       </c>
-      <c r="C32" s="2" t="inlineStr">
+      <c r="C33" s="2" t="inlineStr">
         <is>
           <t>         </t>
         </is>
       </c>
-      <c r="D32" s="2" t="inlineStr">
+      <c r="D33" s="2" t="inlineStr">
         <is>
           <t>        </t>
         </is>
       </c>
-      <c r="E32" s="2" t="inlineStr">
+      <c r="E33" s="2" t="inlineStr">
         <is>
           <t>tierras_aridos</t>
         </is>
       </c>
-      <c r="F32" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G32" s="4" t="n">
+      <c r="F33" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G33" s="4" t="n">
         <v>4.62</v>
       </c>
-      <c r="H32" s="4" t="n">
+      <c r="H33" s="4" t="n">
         <v>1.85</v>
       </c>
-      <c r="I32" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J32" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K32" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L32" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" s="6" t="n">
-        <v>13.88</v>
-      </c>
-      <c r="N32" s="4" t="n">
-        <v>8.33</v>
-      </c>
-      <c r="O32" s="7" t="inlineStr">
+      <c r="I33" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J33" s="2" t="inlineStr">
+        <is>
+          <t>AUMENTAR 19%</t>
+        </is>
+      </c>
+      <c r="K33" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L33" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M33" s="6" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="N33" s="4" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="O33" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
         </is>
       </c>
-      <c r="P32" s="3" t="n">
+      <c r="P33" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="Q32" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S32" s="2" t="n">
+      <c r="Q33" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S33" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="T32" s="3" t="n">
+      <c r="T33" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="U32" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>3203030001</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>ARLITA BOLAS ARCILLA 6L</t>
-        </is>
-      </c>
-      <c r="C33" s="2" t="inlineStr">
-        <is>
-          <t>         </t>
-        </is>
-      </c>
-      <c r="D33" s="2" t="inlineStr">
-        <is>
-          <t>        </t>
-        </is>
-      </c>
-      <c r="E33" s="2" t="inlineStr">
-        <is>
-          <t>tierras_aridos</t>
-        </is>
-      </c>
-      <c r="F33" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" s="4" t="n">
-        <v>9.25</v>
-      </c>
-      <c r="H33" s="4" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="I33" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J33" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K33" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L33" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" s="6" t="n">
-        <v>9.25</v>
-      </c>
-      <c r="N33" s="4" t="n">
-        <v>5.55</v>
-      </c>
-      <c r="O33" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
-        </is>
-      </c>
-      <c r="P33" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="R33" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S33" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="T33" s="3" t="n">
-        <v>2</v>
-      </c>
       <c r="U33" s="8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
+          <t>3203030001</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>ARLITA BOLAS ARCILLA 6L</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>         </t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>        </t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>tierras_aridos</t>
+        </is>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="4" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="I34" s="5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J34" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="6" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="N34" s="4" t="n">
+        <v>5.55</v>
+      </c>
+      <c r="O34" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
+        </is>
+      </c>
+      <c r="P34" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="T34" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="U34" s="8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
           <t>3203030004</t>
         </is>
       </c>
-      <c r="B34" s="2" t="inlineStr">
+      <c r="B35" s="2" t="inlineStr">
         <is>
           <t>PERLITA 5L</t>
         </is>
       </c>
-      <c r="C34" s="2" t="inlineStr">
+      <c r="C35" s="2" t="inlineStr">
         <is>
           <t>         </t>
         </is>
       </c>
-      <c r="D34" s="2" t="inlineStr">
+      <c r="D35" s="2" t="inlineStr">
         <is>
           <t>        </t>
         </is>
       </c>
-      <c r="E34" s="2" t="inlineStr">
+      <c r="E35" s="2" t="inlineStr">
         <is>
           <t>tierras_aridos</t>
         </is>
       </c>
-      <c r="F34" s="3" t="n">
+      <c r="F35" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G34" s="4" t="n">
+      <c r="G35" s="4" t="n">
         <v>5.42</v>
       </c>
-      <c r="H34" s="4" t="n">
+      <c r="H35" s="4" t="n">
         <v>2.17</v>
       </c>
-      <c r="I34" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J34" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K34" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" s="6" t="n">
+      <c r="I35" s="5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J35" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" s="6" t="n">
         <v>10.85</v>
       </c>
-      <c r="N34" s="4" t="n">
+      <c r="N35" s="4" t="n">
         <v>6.51</v>
       </c>
-      <c r="O34" s="7" t="inlineStr">
+      <c r="O35" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">PRODUCTOS FLOWER, S.A.                                                                                                  </t>
         </is>
       </c>
-      <c r="P34" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="3" t="n">
+      <c r="P35" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="R34" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S34" s="2" t="n">
+      <c r="R35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="T34" s="3" t="n">
+      <c r="T35" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="U34" s="8" t="n">
+      <c r="U35" s="8" t="n">
         <v>9</v>
-      </c>
-    </row>
-    <row r="35" hidden="1">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>3101010005</t>
-        </is>
-      </c>
-      <c r="B35" s="2" t="inlineStr">
-        <is>
-          <t>SACO SUSTRATO UNIVERSAL EMUFLOR</t>
-        </is>
-      </c>
-      <c r="C35" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">50L      </t>
-        </is>
-      </c>
-      <c r="D35" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">UNICO   </t>
-        </is>
-      </c>
-      <c r="E35" s="2" t="inlineStr">
-        <is>
-          <t>tierras_aridos</t>
-        </is>
-      </c>
-      <c r="F35" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="G35" s="4" t="n">
-        <v>8.85</v>
-      </c>
-      <c r="H35" s="4" t="n">
-        <v>3.54</v>
-      </c>
-      <c r="I35" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J35" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K35" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="L35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" s="6" t="n">
-        <v>123.9</v>
-      </c>
-      <c r="N35" s="4" t="n">
-        <v>74.34</v>
-      </c>
-      <c r="O35" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SEMILLAS FLORALES, S.L.                                                                                                 </t>
-        </is>
-      </c>
-      <c r="P35" s="3" t="n">
-        <v>105</v>
-      </c>
-      <c r="Q35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="S35" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="T35" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U35" s="8" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="36" hidden="1">
@@ -3360,7 +3360,7 @@
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">70L      </t>
+          <t xml:space="preserve">50L      </t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
@@ -3374,52 +3374,52 @@
         </is>
       </c>
       <c r="F36" s="3" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G36" s="4" t="n">
-        <v>11.8</v>
+        <v>8.85</v>
       </c>
       <c r="H36" s="4" t="n">
-        <v>4.72</v>
+        <v>3.54</v>
       </c>
       <c r="I36" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J36" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K36" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L36" s="3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M36" s="6" t="n">
+        <v>115.05</v>
+      </c>
+      <c r="N36" s="4" t="n">
+        <v>69.03</v>
+      </c>
+      <c r="O36" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEMILLAS FLORALES, S.L.                                                                                                 </t>
+        </is>
+      </c>
+      <c r="P36" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="Q36" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="S36" s="2" t="n">
         <v>3</v>
-      </c>
-      <c r="L36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M36" s="6" t="n">
-        <v>82.59999999999999</v>
-      </c>
-      <c r="N36" s="4" t="n">
-        <v>49.56</v>
-      </c>
-      <c r="O36" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SEMILLAS FLORALES, S.L.                                                                                                 </t>
-        </is>
-      </c>
-      <c r="P36" s="3" t="n">
-        <v>74</v>
-      </c>
-      <c r="Q36" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R36" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="S36" s="2" t="n">
-        <v>0</v>
       </c>
       <c r="T36" s="3" t="n">
         <v>0</v>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="C37" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">20L      </t>
+          <t xml:space="preserve">70L      </t>
         </is>
       </c>
       <c r="D37" s="2" t="inlineStr">
@@ -3455,35 +3455,35 @@
         </is>
       </c>
       <c r="F37" s="3" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G37" s="4" t="n">
-        <v>3.67</v>
+        <v>11.8</v>
       </c>
       <c r="H37" s="4" t="n">
-        <v>1.47</v>
+        <v>4.72</v>
       </c>
       <c r="I37" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J37" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K37" s="3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L37" s="3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M37" s="6" t="n">
-        <v>44.1</v>
+        <v>70.8</v>
       </c>
       <c r="N37" s="4" t="n">
-        <v>26.46</v>
+        <v>42.48</v>
       </c>
       <c r="O37" s="7" t="inlineStr">
         <is>
@@ -3491,16 +3491,16 @@
         </is>
       </c>
       <c r="P37" s="3" t="n">
-        <v>152</v>
+        <v>74</v>
       </c>
       <c r="Q37" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R37" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S37" s="2" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T37" s="3" t="n">
         <v>0</v>
@@ -3512,17 +3512,17 @@
     <row r="38" hidden="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>3102060002</t>
+          <t>3101010005</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>SACO SUSTRATO PLANTAS ACIDOFILAS</t>
+          <t>SACO SUSTRATO UNIVERSAL EMUFLOR</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">45L      </t>
+          <t xml:space="preserve">20L      </t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
@@ -3536,35 +3536,35 @@
         </is>
       </c>
       <c r="F38" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="I38" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J38" s="2" t="inlineStr">
+        <is>
+          <t>AUMENTAR 19%</t>
+        </is>
+      </c>
+      <c r="K38" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="L38" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G38" s="4" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="H38" s="4" t="n">
-        <v>4.12</v>
-      </c>
-      <c r="I38" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J38" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K38" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L38" s="3" t="n">
-        <v>0</v>
-      </c>
       <c r="M38" s="6" t="n">
-        <v>20.6</v>
+        <v>62.47</v>
       </c>
       <c r="N38" s="4" t="n">
-        <v>12.36</v>
+        <v>37.48</v>
       </c>
       <c r="O38" s="7" t="inlineStr">
         <is>
@@ -3572,16 +3572,16 @@
         </is>
       </c>
       <c r="P38" s="3" t="n">
-        <v>43</v>
+        <v>152</v>
       </c>
       <c r="Q38" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R38" s="2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S38" s="2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T38" s="3" t="n">
         <v>0</v>
@@ -3593,22 +3593,22 @@
     <row r="39" hidden="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>3102080001</t>
+          <t>3102060002</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>SACO SUSTRATO COCOPLUS 50L</t>
+          <t>SACO SUSTRATO PLANTAS ACIDOFILAS</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>         </t>
+          <t xml:space="preserve">45L      </t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
         <is>
-          <t>        </t>
+          <t xml:space="preserve">UNICO   </t>
         </is>
       </c>
       <c r="E39" s="2" t="inlineStr">
@@ -3617,22 +3617,22 @@
         </is>
       </c>
       <c r="F39" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G39" s="4" t="n">
-        <v>12.6</v>
+        <v>10.3</v>
       </c>
       <c r="H39" s="4" t="n">
-        <v>5.04</v>
+        <v>4.12</v>
       </c>
       <c r="I39" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J39" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K39" s="3" t="n">
@@ -3642,10 +3642,10 @@
         <v>0</v>
       </c>
       <c r="M39" s="6" t="n">
-        <v>37.8</v>
+        <v>20.6</v>
       </c>
       <c r="N39" s="4" t="n">
-        <v>22.68</v>
+        <v>12.36</v>
       </c>
       <c r="O39" s="7" t="inlineStr">
         <is>
@@ -3653,13 +3653,13 @@
         </is>
       </c>
       <c r="P39" s="3" t="n">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="Q39" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R39" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S39" s="2" t="n">
         <v>0</v>
@@ -3674,12 +3674,12 @@
     <row r="40" hidden="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>3102110003</t>
+          <t>3102080001</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>SACO TIERRA ENRIQUECIDA 50L</t>
+          <t>SACO SUSTRATO COCOPLUS 50L</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
@@ -3698,35 +3698,35 @@
         </is>
       </c>
       <c r="F40" s="3" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G40" s="4" t="n">
-        <v>7.33</v>
+        <v>12.6</v>
       </c>
       <c r="H40" s="4" t="n">
-        <v>2.93</v>
+        <v>5.04</v>
       </c>
       <c r="I40" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J40" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K40" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L40" s="3" t="n">
         <v>0</v>
       </c>
       <c r="M40" s="6" t="n">
-        <v>87.90000000000001</v>
+        <v>37.8</v>
       </c>
       <c r="N40" s="4" t="n">
-        <v>52.74</v>
+        <v>22.68</v>
       </c>
       <c r="O40" s="7" t="inlineStr">
         <is>
@@ -3734,19 +3734,19 @@
         </is>
       </c>
       <c r="P40" s="3" t="n">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="Q40" s="3" t="n">
         <v>0</v>
       </c>
       <c r="R40" s="2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="S40" s="2" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="T40" s="3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U40" s="8" t="n">
         <v>0</v>
@@ -3755,12 +3755,12 @@
     <row r="41" hidden="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>3202030005</t>
+          <t>3102110003</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>SACO MANTILLO SUPER 50L</t>
+          <t>SACO TIERRA ENRIQUECIDA 50L</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
@@ -3779,55 +3779,55 @@
         </is>
       </c>
       <c r="F41" s="3" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G41" s="4" t="n">
-        <v>5.47</v>
+        <v>7.33</v>
       </c>
       <c r="H41" s="4" t="n">
-        <v>2.19</v>
+        <v>2.93</v>
       </c>
       <c r="I41" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J41" s="2" t="inlineStr">
         <is>
-          <t>MANTENER</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K41" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="L41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="6" t="n">
+        <v>80.58</v>
+      </c>
+      <c r="N41" s="4" t="n">
+        <v>48.35</v>
+      </c>
+      <c r="O41" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEMILLAS FLORALES, S.L.                                                                                                 </t>
+        </is>
+      </c>
+      <c r="P41" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="Q41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="L41" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" s="6" t="n">
-        <v>98.55</v>
-      </c>
-      <c r="N41" s="4" t="n">
-        <v>59.13</v>
-      </c>
-      <c r="O41" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SEMILLAS FLORALES, S.L.                                                                                                 </t>
-        </is>
-      </c>
-      <c r="P41" s="3" t="n">
-        <v>161</v>
-      </c>
-      <c r="Q41" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" s="2" t="n">
-        <v>4</v>
-      </c>
       <c r="S41" s="2" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="T41" s="3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U41" s="8" t="n">
         <v>0</v>
@@ -3836,306 +3836,387 @@
     <row r="42" hidden="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
+          <t>3202030005</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>SACO MANTILLO SUPER 50L</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>         </t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>        </t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>tierras_aridos</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="G42" s="4" t="n">
+        <v>5.47</v>
+      </c>
+      <c r="H42" s="4" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="I42" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J42" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K42" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L42" s="3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="M42" s="6" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="N42" s="4" t="n">
+        <v>52.56</v>
+      </c>
+      <c r="O42" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SEMILLAS FLORALES, S.L.                                                                                                 </t>
+        </is>
+      </c>
+      <c r="P42" s="3" t="n">
+        <v>161</v>
+      </c>
+      <c r="Q42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="S42" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="T42" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U42" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" hidden="1">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
           <t>3203030002</t>
         </is>
       </c>
-      <c r="B42" s="2" t="inlineStr">
+      <c r="B43" s="2" t="inlineStr">
         <is>
           <t>SACO ARLITA 15L</t>
         </is>
       </c>
-      <c r="C42" s="2" t="inlineStr">
+      <c r="C43" s="2" t="inlineStr">
         <is>
           <t>         </t>
         </is>
       </c>
-      <c r="D42" s="2" t="inlineStr">
+      <c r="D43" s="2" t="inlineStr">
         <is>
           <t>        </t>
         </is>
       </c>
-      <c r="E42" s="2" t="inlineStr">
+      <c r="E43" s="2" t="inlineStr">
         <is>
           <t>tierras_aridos</t>
         </is>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F43" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G42" s="4" t="n">
+      <c r="G43" s="4" t="n">
         <v>11.33</v>
       </c>
-      <c r="H42" s="4" t="n">
+      <c r="H43" s="4" t="n">
         <v>4.53</v>
       </c>
-      <c r="I42" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J42" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K42" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L42" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M42" s="6" t="n">
+      <c r="I43" s="5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="J43" s="2" t="inlineStr">
+        <is>
+          <t>REDUCIR 19%</t>
+        </is>
+      </c>
+      <c r="K43" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" s="6" t="n">
         <v>22.65</v>
       </c>
-      <c r="N42" s="4" t="n">
+      <c r="N43" s="4" t="n">
         <v>13.59</v>
       </c>
-      <c r="O42" s="7" t="inlineStr">
+      <c r="O43" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">SEMILLAS FLORALES, S.L.                                                                                                 </t>
         </is>
       </c>
-      <c r="P42" s="3" t="n">
+      <c r="P43" s="3" t="n">
         <v>66</v>
       </c>
-      <c r="Q42" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T42" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U42" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="inlineStr">
+      <c r="Q43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T43" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U43" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>3201020000</t>
         </is>
       </c>
-      <c r="B43" s="2" t="inlineStr">
+      <c r="B44" s="2" t="inlineStr">
         <is>
           <t>BIG BAG MANTILLO 500L (*)</t>
         </is>
       </c>
-      <c r="C43" s="2" t="inlineStr">
+      <c r="C44" s="2" t="inlineStr">
         <is>
           <t>         </t>
         </is>
       </c>
-      <c r="D43" s="2" t="inlineStr">
+      <c r="D44" s="2" t="inlineStr">
         <is>
           <t>        </t>
         </is>
       </c>
-      <c r="E43" s="2" t="inlineStr">
+      <c r="E44" s="2" t="inlineStr">
         <is>
           <t>tierras_aridos</t>
         </is>
       </c>
-      <c r="F43" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G43" s="4" t="n">
+      <c r="F44" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G44" s="4" t="n">
         <v>59.1</v>
       </c>
-      <c r="H43" s="4" t="n">
+      <c r="H44" s="4" t="n">
         <v>23.64</v>
       </c>
-      <c r="I43" s="5" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="J43" s="2" t="inlineStr">
-        <is>
-          <t>MANTENER</t>
-        </is>
-      </c>
-      <c r="K43" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L43" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M43" s="6" t="n">
-        <v>177.3</v>
-      </c>
-      <c r="N43" s="4" t="n">
-        <v>106.38</v>
-      </c>
-      <c r="O43" s="7" t="inlineStr">
+      <c r="I44" s="5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J44" s="2" t="inlineStr">
+        <is>
+          <t>AUMENTAR 19%</t>
+        </is>
+      </c>
+      <c r="K44" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L44" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M44" s="6" t="n">
+        <v>236.4</v>
+      </c>
+      <c r="N44" s="4" t="n">
+        <v>141.84</v>
+      </c>
+      <c r="O44" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">SURGE AMBIENTAL SL                                                                                                      </t>
         </is>
       </c>
-      <c r="P43" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="R43" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S43" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T43" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="U43" s="8" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44"/>
-    <row r="45">
-      <c r="B45" s="9" t="inlineStr">
+      <c r="P44" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="R44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S44" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T44" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U44" s="8" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45"/>
+    <row r="46">
+      <c r="B46" s="9" t="inlineStr">
         <is>
           <t>METRICAS DE RESUMEN</t>
         </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" s="10" t="inlineStr">
-        <is>
-          <t>Total_Unidades:</t>
-        </is>
-      </c>
-      <c r="C46" s="5" t="n">
-        <v>36</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="10" t="inlineStr">
         <is>
-          <t>Total_Articulos:</t>
+          <t>Total_Unidades:</t>
         </is>
       </c>
       <c r="C47" s="5" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="10" t="inlineStr">
         <is>
-          <t>Total_Importe:</t>
-        </is>
-      </c>
-      <c r="C48" s="5" t="inlineStr">
-        <is>
-          <t>1757.10€</t>
-        </is>
+          <t>Total_Articulos:</t>
+        </is>
+      </c>
+      <c r="C48" s="5" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" s="10" t="inlineStr">
         <is>
-          <t>Objetivo_Semana:</t>
+          <t>Total_Importe:</t>
         </is>
       </c>
       <c r="C49" s="5" t="inlineStr">
         <is>
-          <t>1664.45€</t>
+          <t>1748.30€</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="10" t="inlineStr">
         <is>
-          <t>Factor_Crecimiento:</t>
+          <t>Objetivo_Semana:</t>
         </is>
       </c>
       <c r="C50" s="5" t="inlineStr">
         <is>
-          <t>5%</t>
+          <t>1664.45€</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="10" t="inlineStr">
         <is>
-          <t>Factor_Festivo:</t>
+          <t>Factor_Crecimiento:</t>
         </is>
       </c>
       <c r="C51" s="5" t="inlineStr">
         <is>
-          <t>0%</t>
+          <t>5%</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="10" t="inlineStr">
         <is>
-          <t>Articulos_A:</t>
-        </is>
-      </c>
-      <c r="C52" s="5" t="n">
-        <v>0</v>
+          <t>Factor_Festivo:</t>
+        </is>
+      </c>
+      <c r="C52" s="5" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
     </row>
     <row r="53">
       <c r="B53" s="10" t="inlineStr">
         <is>
-          <t>Articulos_B:</t>
+          <t>Articulos_A:</t>
         </is>
       </c>
       <c r="C53" s="5" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" s="10" t="inlineStr">
         <is>
-          <t>Articulos_C:</t>
+          <t>Articulos_B:</t>
         </is>
       </c>
       <c r="C54" s="5" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="10" t="inlineStr">
         <is>
-          <t>Stock_Minimo_%:</t>
-        </is>
-      </c>
-      <c r="C55" s="5" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
+          <t>Articulos_C:</t>
+        </is>
+      </c>
+      <c r="C55" s="5" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="10" t="inlineStr">
         <is>
-          <t>Stock_Minimo_Objetivo:</t>
-        </is>
-      </c>
-      <c r="C56" s="5" t="n">
-        <v>95</v>
+          <t>Stock_Minimo_%:</t>
+        </is>
+      </c>
+      <c r="C56" s="5" t="inlineStr">
+        <is>
+          <t>30%</t>
+        </is>
       </c>
     </row>
     <row r="57">
       <c r="B57" s="10" t="inlineStr">
         <is>
+          <t>Stock_Minimo_Objetivo:</t>
+        </is>
+      </c>
+      <c r="C57" s="5" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="10" t="inlineStr">
+        <is>
           <t>Total_Ajuste_Stock:</t>
         </is>
       </c>
-      <c r="C57" s="5" t="n">
-        <v>0</v>
+      <c r="C58" s="5" t="n">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0.2" bottom="0.2" header="0" footer="0"/>
   <pageSetup orientation="landscape" fitToHeight="0" fitToWidth="1"/>

</xml_diff>